<commit_message>
Déplacements message quand on /duel player dans Demande_Duel
</commit_message>
<xml_diff>
--- a/dependances_commandes_duel.xlsx
+++ b/dependances_commandes_duel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\Programmation_JAVA\IntelliJ\duels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19434C6-56BB-44BF-BA56-ABBE80A4F5C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04148950-3BC4-442C-9EEC-05E502E99A69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2B65277-D444-4199-B7F4-5D02EE67EAF1}"/>
   </bookViews>
@@ -33,8 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1766841A-70C5-4EBA-9D9C-16E0F1E5D74C}</author>
+  </authors>
+  <commentList>
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{1766841A-70C5-4EBA-9D9C-16E0F1E5D74C}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    TODO : Les duels le concernant</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>rien</t>
   </si>
@@ -121,13 +139,16 @@
   </si>
   <si>
     <t>La fonction a bien été codée.</t>
+  </si>
+  <si>
+    <t>On donne les infos puis on renvoie la liste des duels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +178,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -262,19 +289,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -301,6 +315,21 @@
       </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -855,7 +884,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -869,214 +898,193 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1138,6 +1146,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="49" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1528,6 +1551,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ylane T" id="{AAC842DA-F158-450C-B122-7D41AEE4F41B}" userId="Ylane T" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -1823,15 +1852,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="L8" dT="2020-10-24T15:44:56.40" personId="{AAC842DA-F158-450C-B122-7D41AEE4F41B}" id="{1766841A-70C5-4EBA-9D9C-16E0F1E5D74C}">
+    <text>TODO : Les duels le concernant</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE7F9AB-BECA-4A9E-94BD-05F0CDAF047B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE7F9AB-BECA-4A9E-94BD-05F0CDAF047B}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,79 +1882,79 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="63"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="56"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="78"/>
-      <c r="N3" s="75" t="s">
+      <c r="M3" s="71"/>
+      <c r="N3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="77"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="70"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="69" t="s">
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="70" t="s">
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70" t="s">
+      <c r="M4" s="63"/>
+      <c r="N4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="70"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="70"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="63"/>
     </row>
     <row r="5" spans="1:18" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
@@ -1950,10 +1987,10 @@
       <c r="K5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="79" t="s">
+      <c r="M5" s="72" t="s">
         <v>16</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -1976,93 +2013,95 @@
       <c r="A6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="68"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="61"/>
     </row>
     <row r="7" spans="1:18" ht="53.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="43" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="43" t="s">
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
-      <c r="R7" s="56"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="49"/>
     </row>
     <row r="8" spans="1:18" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="55"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="92"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
     </row>
     <row r="9" spans="1:18" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="37" t="s">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="89" t="s">
         <v>22</v>
       </c>
       <c r="M9" s="17"/>
@@ -2076,20 +2115,20 @@
       <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="32"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="17"/>
       <c r="N10" s="18"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
@@ -2100,46 +2139,46 @@
       <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="35"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="33"/>
     </row>
     <row r="12" spans="1:18" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
       <c r="G12" s="22"/>
       <c r="H12" s="21"/>
       <c r="I12" s="23"/>
       <c r="J12" s="24"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="31"/>
+      <c r="M12" s="91"/>
       <c r="N12" s="20"/>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
@@ -2147,56 +2186,56 @@
       <c r="R12" s="9"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
     </row>
     <row r="17" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
     </row>
     <row r="18" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="32">
@@ -2235,6 +2274,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2248,69 +2288,69 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="15.7109375" style="93" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="93"/>
+    <col min="1" max="26" width="15.7109375" style="86" customWidth="1"/>
+    <col min="27" max="16384" width="11.42578125" style="86"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="85"/>
-      <c r="B1" s="64" t="s">
+      <c r="A1" s="78"/>
+      <c r="B1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="86"/>
-      <c r="B2" s="66" t="s">
+      <c r="A2" s="79"/>
+      <c r="B2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="87"/>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="80"/>
+      <c r="B3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
-      <c r="B4" s="53" t="s">
+      <c r="A4" s="81"/>
+      <c r="B4" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="81" t="s">
+      <c r="A5" s="82"/>
+      <c r="B5" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="82"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="75"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="90"/>
-      <c r="B6" s="83" t="s">
+      <c r="A6" s="83"/>
+      <c r="B6" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="77"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -2321,129 +2361,129 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="91"/>
-      <c r="B8" s="94" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="94"/>
+      <c r="C8" s="87"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="91"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="87"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="91"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
+      <c r="A11" s="84"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
+      <c r="A12" s="84"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="91"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
+      <c r="A13" s="84"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="92"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="85"/>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="92"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="92"/>
-      <c r="E21" s="92"/>
-      <c r="F21" s="92"/>
-      <c r="G21" s="92"/>
-      <c r="H21" s="92"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="92"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="92"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>